<commit_message>
add console log for kanji or word. Kanji url is currently not working.
</commit_message>
<xml_diff>
--- a/kanji.xlsx
+++ b/kanji.xlsx
@@ -19,69 +19,40 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Kanji</t>
-  </si>
-  <si>
-    <t>おふくろ</t>
-  </si>
-  <si>
-    <t>郷愁</t>
-  </si>
-  <si>
-    <t>世</t>
   </si>
   <si>
     <t>幾</t>
   </si>
   <si>
-    <t>油揚げ</t>
+    <t>郷</t>
   </si>
   <si>
-    <t>要する</t>
+    <t>愁</t>
   </si>
   <si>
-    <t>注ぐ</t>
-  </si>
-  <si>
-    <t>言</t>
-  </si>
-  <si>
-    <t>作り</t>
-  </si>
-  <si>
-    <t>中略</t>
-  </si>
-  <si>
-    <t>甚だ</t>
-  </si>
-  <si>
-    <t>流動</t>
-  </si>
-  <si>
-    <t>密着</t>
-  </si>
-  <si>
-    <t>漂白</t>
-  </si>
-  <si>
-    <t>だし</t>
-  </si>
-  <si>
-    <t>味気ない</t>
+    <t>要</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -133,14 +104,15 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -419,7 +391,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A17"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4"/>
@@ -456,7 +428,7 @@
     </row>
     <row r="2" spans="1:26">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -486,7 +458,7 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
@@ -516,7 +488,7 @@
     </row>
     <row r="4" spans="1:26">
       <c r="A4" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
@@ -575,9 +547,6 @@
       <c r="Z5" s="2"/>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
       <c r="B6" s="2"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
@@ -605,9 +574,6 @@
       <c r="Z6" s="2"/>
     </row>
     <row r="7" spans="1:26">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
@@ -635,9 +601,6 @@
       <c r="Z7" s="2"/>
     </row>
     <row r="8" spans="1:26">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
@@ -665,9 +628,6 @@
       <c r="Z8" s="2"/>
     </row>
     <row r="9" spans="1:26">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
@@ -695,9 +655,6 @@
       <c r="Z9" s="2"/>
     </row>
     <row r="10" spans="1:26">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
@@ -725,9 +682,6 @@
       <c r="Z10" s="2"/>
     </row>
     <row r="11" spans="1:26">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
@@ -755,9 +709,6 @@
       <c r="Z11" s="2"/>
     </row>
     <row r="12" spans="1:26">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
@@ -785,9 +736,7 @@
       <c r="Z12" s="2"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
+      <c r="A13" s="3"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
@@ -815,9 +764,6 @@
       <c r="Z13" s="2"/>
     </row>
     <row r="14" spans="1:26">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
@@ -845,9 +791,7 @@
       <c r="Z14" s="2"/>
     </row>
     <row r="15" spans="1:26">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
+      <c r="A15" s="3"/>
       <c r="B15" s="2"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
@@ -875,9 +819,6 @@
       <c r="Z15" s="2"/>
     </row>
     <row r="16" spans="1:26">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
       <c r="B16" s="2"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
@@ -904,10 +845,7 @@
       <c r="Y16" s="2"/>
       <c r="Z16" s="2"/>
     </row>
-    <row r="17" spans="1:26">
-      <c r="A17" t="s">
-        <v>16</v>
-      </c>
+    <row r="17" spans="2:26">
       <c r="B17" s="2"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
@@ -934,7 +872,7 @@
       <c r="Y17" s="2"/>
       <c r="Z17" s="2"/>
     </row>
-    <row r="18" spans="1:26">
+    <row r="18" spans="2:26">
       <c r="B18" s="2"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
@@ -961,7 +899,7 @@
       <c r="Y18" s="2"/>
       <c r="Z18" s="2"/>
     </row>
-    <row r="19" spans="1:26">
+    <row r="19" spans="2:26">
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
@@ -988,7 +926,7 @@
       <c r="Y19" s="2"/>
       <c r="Z19" s="2"/>
     </row>
-    <row r="20" spans="1:26">
+    <row r="20" spans="2:26">
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
@@ -1015,7 +953,7 @@
       <c r="Y20" s="2"/>
       <c r="Z20" s="2"/>
     </row>
-    <row r="21" spans="1:26">
+    <row r="21" spans="2:26">
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
@@ -1042,7 +980,7 @@
       <c r="Y21" s="2"/>
       <c r="Z21" s="2"/>
     </row>
-    <row r="22" spans="1:26">
+    <row r="22" spans="2:26">
       <c r="B22" s="2"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
@@ -1069,7 +1007,7 @@
       <c r="Y22" s="2"/>
       <c r="Z22" s="2"/>
     </row>
-    <row r="23" spans="1:26">
+    <row r="23" spans="2:26">
       <c r="B23" s="2"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
@@ -1096,7 +1034,7 @@
       <c r="Y23" s="2"/>
       <c r="Z23" s="2"/>
     </row>
-    <row r="24" spans="1:26">
+    <row r="24" spans="2:26">
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
@@ -1123,7 +1061,7 @@
       <c r="Y24" s="2"/>
       <c r="Z24" s="2"/>
     </row>
-    <row r="25" spans="1:26">
+    <row r="25" spans="2:26">
       <c r="B25" s="2"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
@@ -1150,7 +1088,7 @@
       <c r="Y25" s="2"/>
       <c r="Z25" s="2"/>
     </row>
-    <row r="26" spans="1:26">
+    <row r="26" spans="2:26">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
@@ -1177,7 +1115,7 @@
       <c r="Y26" s="2"/>
       <c r="Z26" s="2"/>
     </row>
-    <row r="27" spans="1:26">
+    <row r="27" spans="2:26">
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
@@ -1204,7 +1142,7 @@
       <c r="Y27" s="2"/>
       <c r="Z27" s="2"/>
     </row>
-    <row r="28" spans="1:26">
+    <row r="28" spans="2:26">
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
@@ -1231,7 +1169,7 @@
       <c r="Y28" s="2"/>
       <c r="Z28" s="2"/>
     </row>
-    <row r="29" spans="1:26">
+    <row r="29" spans="2:26">
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
@@ -1258,7 +1196,7 @@
       <c r="Y29" s="2"/>
       <c r="Z29" s="2"/>
     </row>
-    <row r="30" spans="1:26">
+    <row r="30" spans="2:26">
       <c r="B30" s="2"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
@@ -1285,7 +1223,7 @@
       <c r="Y30" s="2"/>
       <c r="Z30" s="2"/>
     </row>
-    <row r="31" spans="1:26">
+    <row r="31" spans="2:26">
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
@@ -1312,7 +1250,7 @@
       <c r="Y31" s="2"/>
       <c r="Z31" s="2"/>
     </row>
-    <row r="32" spans="1:26">
+    <row r="32" spans="2:26">
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
       <c r="D32" s="2"/>
@@ -27948,5 +27886,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>